<commit_message>
Commit 1: Nuevo registro
opcion 2 funcional, se registra un nuevo libro
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>No</t>
   </si>
@@ -123,6 +123,24 @@
   </si>
   <si>
     <t>j. r. tolkien</t>
+  </si>
+  <si>
+    <t>juancito</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>libro</t>
+  </si>
+  <si>
+    <t>autor</t>
+  </si>
+  <si>
+    <t>azul</t>
+  </si>
+  <si>
+    <t>verde</t>
   </si>
 </sst>
 </file>
@@ -475,7 +493,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="D2">
         <v>20</v>
@@ -531,7 +549,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="D6">
         <v>52</v>
@@ -661,6 +679,34 @@
       </c>
       <c r="D15" t="n">
         <v>41.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="n">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="n">
+        <v>500.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit 2: Nuevo registro-Valida 30
Valida que solo puedan haber 30 registros, crea nuevas sheet al llegar a 30 registros
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ficheros-Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="8625" windowWidth="12210" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12210" windowHeight="8625" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Java Books" r:id="rId1" sheetId="1"/>
+    <sheet name="Java Books" sheetId="1" r:id="rId1"/>
+    <sheet name="Java Books 1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>No</t>
   </si>
@@ -56,21 +52,12 @@
     <t>El fin de la dictadura</t>
   </si>
   <si>
-    <t>Juan Stand</t>
-  </si>
-  <si>
-    <t>Luisa Pedroza</t>
-  </si>
-  <si>
     <t>Ana Matia Mujica</t>
   </si>
   <si>
     <t>Kuan Hg</t>
   </si>
   <si>
-    <t>Jhon Ricardo</t>
-  </si>
-  <si>
     <t>Juan G.</t>
   </si>
   <si>
@@ -141,13 +128,21 @@
   </si>
   <si>
     <t>verde</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>ert</t>
+  </si>
+  <si>
+    <t>ger</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -175,16 +170,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -201,10 +196,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -239,7 +234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -274,7 +269,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -368,21 +363,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -399,7 +394,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -451,24 +446,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -493,7 +488,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D2">
         <v>20</v>
@@ -507,10 +502,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="n">
-        <v>300.0</v>
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -521,7 +516,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>78</v>
@@ -535,7 +530,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>102</v>
@@ -549,7 +544,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>52</v>
@@ -563,153 +558,404 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>500</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7.0</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="n">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="n">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="D10" t="n">
-        <v>32.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="n">
-        <v>41.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C13" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="n">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C14" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>27</v>
       </c>
-      <c r="D13" t="n">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C15" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D15">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="D14" t="n">
-        <v>32.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="C15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" t="n">
-        <v>41.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>36</v>
       </c>
-      <c r="D16" t="n">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>16.0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="D17" t="n">
-        <v>500.0</v>
+      <c r="D3">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregada la parte del Alumno C
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>No</t>
   </si>
@@ -96,6 +96,33 @@
   </si>
   <si>
     <t>Jez Humble</t>
+  </si>
+  <si>
+    <t>El que se duerme pierde</t>
+  </si>
+  <si>
+    <t>Tom Peter</t>
+  </si>
+  <si>
+    <t>Sin lugar a duda</t>
+  </si>
+  <si>
+    <t>Ana Gutierrez</t>
+  </si>
+  <si>
+    <t>El arte de dormir</t>
+  </si>
+  <si>
+    <t>Nico</t>
+  </si>
+  <si>
+    <t>Buscando a Nemo</t>
+  </si>
+  <si>
+    <t>Humble Po</t>
+  </si>
+  <si>
+    <t>j. r. tolkien</t>
   </si>
 </sst>
 </file>
@@ -422,8 +449,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.28515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.28515625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -462,10 +489,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="D3" t="n">
+        <v>300.0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -577,6 +604,62 @@
         <v>23</v>
       </c>
       <c r="D11" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="n">
         <v>41.0</v>
       </c>
     </row>

</xml_diff>